<commit_message>
Add real data for fuel use reduction and capital cost of electrifying low-temp industrial heat with heat pumps (#196)
</commit_message>
<xml_diff>
--- a/InputData/indst/PIFURfE/Perc Indst Fuel Use Reduction for Elec.xlsx
+++ b/InputData/indst/PIFURfE/Perc Indst Fuel Use Reduction for Elec.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\PIFURfE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13ED131B-5805-4322-8338-AD35EEC5EF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B41C68-DFE6-4CD7-B6F4-92A8676F4F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13515" yWindow="1275" windowWidth="26865" windowHeight="20775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11070" yWindow="0" windowWidth="32460" windowHeight="18330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Table 5.2" sheetId="4" r:id="rId2"/>
-    <sheet name="Calculations" sheetId="5" r:id="rId3"/>
-    <sheet name="PIFURfE" sheetId="2" r:id="rId4"/>
+    <sheet name="Med-High Temp Heat" sheetId="5" r:id="rId3"/>
+    <sheet name="Low Temp Heat" sheetId="6" r:id="rId4"/>
+    <sheet name="PIFURfE" sheetId="2" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_Regression_Int" localSheetId="1" hidden="1">1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Table 5.2'!$A$1:$J$1921</definedName>
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8870" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8912" uniqueCount="339">
   <si>
     <t>Percentage Industry Fuel Use Reduction for Electricity</t>
   </si>
@@ -969,7 +973,106 @@
     <t>medium and high temperature</t>
   </si>
   <si>
-    <t>Add data and sourcing for temperature disaggregation</t>
+    <t>Temp Increase (°C)</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>Arpagaus, Cordin et al.</t>
+  </si>
+  <si>
+    <t>High Temperature Heat Pumps: Market Overview, State of the Art, Research Status, Refrigerants, and Application Potentials</t>
+  </si>
+  <si>
+    <t>https://docs.lib.purdue.edu/cgi/viewcontent.cgi?article=2875&amp;context=iracc</t>
+  </si>
+  <si>
+    <t>Industrial Heat Pump Efficiency</t>
+  </si>
+  <si>
+    <t>Room Temperature</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Temp Need for Low-Temp Heat</t>
+  </si>
+  <si>
+    <t>See variable indst/IHDbT</t>
+  </si>
+  <si>
+    <t>The low-temp heat range represents the heat that can be delivered by industrial heat pumps,</t>
+  </si>
+  <si>
+    <t>i.e., up to about 150-165 C.  This represents around 30% of the total bar height in IHDbT.</t>
+  </si>
+  <si>
+    <t>Of that 30%:</t>
+  </si>
+  <si>
+    <t>We assume the average heat need in the &lt;100 C category is:</t>
+  </si>
+  <si>
+    <t>We assume the average heat need in the 100 to 165 C category is:</t>
+  </si>
+  <si>
+    <t>The weighted average temperature requirement among low-temp processes is:</t>
+  </si>
+  <si>
+    <t>percentage points are &lt;100 C.</t>
+  </si>
+  <si>
+    <t>percentage points range from 100 to 165 C.</t>
+  </si>
+  <si>
+    <t>This corresponds to a temperature increase (relative to a room temp heat sink) of:</t>
+  </si>
+  <si>
+    <t>This corresponds to a coefficient of performance (according to graph at right) of about:</t>
+  </si>
+  <si>
+    <t>A boiler represents a fairly typical piece of industrial equipment that often delivers</t>
+  </si>
+  <si>
+    <t>low-temperature heat.  Here are some statistics on fossil boiler efficiency from U.S. DOE:</t>
+  </si>
+  <si>
+    <t>Fossil Fuel Equipment Efficiency</t>
+  </si>
+  <si>
+    <t>We will use the mid-tier to represent a typical boiler that would be replaced with electric.</t>
+  </si>
+  <si>
+    <t>To deliver 1 unit of heat, the fossil fuel boiler needs:</t>
+  </si>
+  <si>
+    <t>units of energy</t>
+  </si>
+  <si>
+    <t>To deliver one unit of heat, the heat pump needs:</t>
+  </si>
+  <si>
+    <t>Therefore, the percent energy use reduction from switching is:</t>
+  </si>
+  <si>
+    <t>Low temp electrical heat is provided by heat pumps.</t>
+  </si>
+  <si>
+    <t>Heat pumps have a range of efficiencies depending on the amount of temperature increase they deliver.</t>
+  </si>
+  <si>
+    <t>Medium and High-Temp electrical heat can be provided by a range of technologies, such as</t>
+  </si>
+  <si>
+    <t>induction, electric resistance, infrared, dielectric heating, etc.</t>
+  </si>
+  <si>
+    <t>For low-temperature industrial heat, we use industrial heat pumps.</t>
+  </si>
+  <si>
+    <t>We will use some representative technologies below to form our estimate.</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1084,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1055,8 +1158,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1072,12 +1191,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,13 +1231,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1205,10 +1319,21 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
@@ -1225,6 +1350,2821 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Low Temp Heat'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="31750">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Low Temp Heat'!$A$5:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>56.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>84.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Low Temp Heat'!$B$5:$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F89E-481B-8A06-51EB1A1DD5A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1808965472"/>
+        <c:axId val="1808962144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1808965472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1808962144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1808962144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1808965472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Industrial Heat Pump Efficiency vs. Delivered</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> Temperature Increase</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Low Temp Heat'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Low Temp Heat'!$A$5:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>56.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>84.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Low Temp Heat'!$B$5:$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5C27-49BD-A190-E44C93998AE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2005302688"/>
+        <c:axId val="2005298112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2005302688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Temperature Increase (°C)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2005298112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2005298112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Coefficient of Performance (COP)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.1590044939753746E-3"/>
+              <c:y val="0.24265854338040146"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2005302688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>20292</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>168551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>477493</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>69684</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE7CBCCD-4900-470E-BA07-C511D1972A37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2631263" y="168551"/>
+          <a:ext cx="7718612" cy="7140133"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>329852</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>151881</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>229843</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>130450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CC9ED2A-445F-4E79-9491-62E66D5F2D4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>13485</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>178538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>247688</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>140438</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DFDDFCA-1A6E-4A33-8F40-5AD5479E6B9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>COP</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>25</v>
+          </cell>
+          <cell r="B2">
+            <v>5.77</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>30</v>
+          </cell>
+          <cell r="B3">
+            <v>4.99</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>35</v>
+          </cell>
+          <cell r="B4">
+            <v>4.01</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>40</v>
+          </cell>
+          <cell r="B5">
+            <v>4.71</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>40</v>
+          </cell>
+          <cell r="B6">
+            <v>4.25</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>40</v>
+          </cell>
+          <cell r="B7">
+            <v>4.05</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>40</v>
+          </cell>
+          <cell r="B8">
+            <v>3.95</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>40</v>
+          </cell>
+          <cell r="B9">
+            <v>3.66</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>40</v>
+          </cell>
+          <cell r="B10">
+            <v>3.39</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>45</v>
+          </cell>
+          <cell r="B11">
+            <v>4.9800000000000004</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>45.2</v>
+          </cell>
+          <cell r="B12">
+            <v>3.99</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>50</v>
+          </cell>
+          <cell r="B13">
+            <v>4.0999999999999996</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>50.8</v>
+          </cell>
+          <cell r="B14">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>50</v>
+          </cell>
+          <cell r="B15">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>50</v>
+          </cell>
+          <cell r="B16">
+            <v>3.6</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>50</v>
+          </cell>
+          <cell r="B17">
+            <v>3.35</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>50</v>
+          </cell>
+          <cell r="B18">
+            <v>3.1</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>50</v>
+          </cell>
+          <cell r="B19">
+            <v>2.98</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>55</v>
+          </cell>
+          <cell r="B20">
+            <v>3.5</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>55</v>
+          </cell>
+          <cell r="B21">
+            <v>2.7</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>56.4</v>
+          </cell>
+          <cell r="B22">
+            <v>3.6</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>60.2</v>
+          </cell>
+          <cell r="B23">
+            <v>4.5</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>60</v>
+          </cell>
+          <cell r="B24">
+            <v>2.89</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>60</v>
+          </cell>
+          <cell r="B25">
+            <v>2.75</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>60</v>
+          </cell>
+          <cell r="B26">
+            <v>2.06</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>63.2</v>
+          </cell>
+          <cell r="B27">
+            <v>2.69</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>61.4</v>
+          </cell>
+          <cell r="B28">
+            <v>3.45</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>65</v>
+          </cell>
+          <cell r="B29">
+            <v>3.1</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>70</v>
+          </cell>
+          <cell r="B30">
+            <v>2.6</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>75</v>
+          </cell>
+          <cell r="B31">
+            <v>2.7</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>75</v>
+          </cell>
+          <cell r="B32">
+            <v>2.37</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>80</v>
+          </cell>
+          <cell r="B33">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>84.7</v>
+          </cell>
+          <cell r="B34">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>90</v>
+          </cell>
+          <cell r="B35">
+            <v>1.98</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>95</v>
+          </cell>
+          <cell r="B36">
+            <v>2.48</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>95</v>
+          </cell>
+          <cell r="B37">
+            <v>1.98</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>100</v>
+          </cell>
+          <cell r="B38">
+            <v>1.69</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>105</v>
+          </cell>
+          <cell r="B39">
+            <v>2.19</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>115</v>
+          </cell>
+          <cell r="B40">
+            <v>1.98</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>130</v>
+          </cell>
+          <cell r="B41">
+            <v>1.58</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1548,7 +4488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1645,43 +4585,70 @@
         <v>284</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="32" t="s">
+        <v>310</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="33">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="45" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="43" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
-        <v>305</v>
-      </c>
-      <c r="B30" s="45"/>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B26" r:id="rId1" xr:uid="{AE0B3FDC-7092-4F02-BB35-56CA5D290868}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -52719,7 +55686,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -52730,190 +55697,782 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="38"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="36">
+      <c r="B5" s="38"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
         <f>AVERAGE(0.56,0.7)</f>
         <v>0.63</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="42">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="42">
         <f>AVERAGE(0.8,0.83)</f>
         <v>0.81499999999999995</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
         <f>AVERAGE(0.9,0.985)</f>
         <v>0.9425</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
         <f>AVERAGE(0.95,1)</f>
         <v>0.97499999999999998</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
-        <f>(A5-A3)/A3</f>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="39">
+        <f>(A9-A7)/A7</f>
         <v>0.19631901840490804</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="B14" s="38"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B18" s="38"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="34">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
         <v>0.2</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B23" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="34">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="34">
         <v>0.35</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="34">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="34">
         <v>0.6</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="34">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="34">
         <v>0.8</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B26" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="40">
-        <f>1-A20</f>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
+        <f>1-A24</f>
         <v>0.65</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B31" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="B29" s="38"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B33" s="38"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="37">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="37">
         <f>SUM('Table 5.2'!E20:I20,'Table 5.2'!E24:I24,'Table 5.2'!E30:I30)/SUM('Table 5.2'!E20:I20,'Table 5.2'!E23:I23,'Table 5.2'!E29:I29)</f>
         <v>0.92744126578232378</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B36" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="37">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="37">
         <f>SUM('Table 5.2'!E25:I28,'Table 5.2'!E31:I35)/SUM('Table 5.2'!E20:I20,'Table 5.2'!E23:I23,'Table 5.2'!E29:I29)</f>
         <v>7.1439987214319961E-2</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="41">
-        <f>A32*A11+A33*A27</f>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="41">
+        <f>A36*A15+A37*A31</f>
         <v>0.22851035061589922</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B39" t="s">
         <v>299</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A32:A33" formulaRange="1"/>
+    <ignoredError sqref="A36:A37" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E954BD9-F2E9-49BD-A674-73E808A9938A}">
+  <dimension ref="A1:B95"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>4.9800000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>45.2</v>
+      </c>
+      <c r="B15">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>50.8</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>50</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>55</v>
+      </c>
+      <c r="B23">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>55</v>
+      </c>
+      <c r="B24">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>56.4</v>
+      </c>
+      <c r="B25">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>60.2</v>
+      </c>
+      <c r="B26">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>60</v>
+      </c>
+      <c r="B27">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>60</v>
+      </c>
+      <c r="B28">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>60</v>
+      </c>
+      <c r="B29">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>63.2</v>
+      </c>
+      <c r="B30">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>61.4</v>
+      </c>
+      <c r="B31">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>65</v>
+      </c>
+      <c r="B32">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>70</v>
+      </c>
+      <c r="B33">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>75</v>
+      </c>
+      <c r="B34">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>75</v>
+      </c>
+      <c r="B35">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>80</v>
+      </c>
+      <c r="B36">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>84.7</v>
+      </c>
+      <c r="B37">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>90</v>
+      </c>
+      <c r="B38">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>95</v>
+      </c>
+      <c r="B39">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>95</v>
+      </c>
+      <c r="B40">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>100</v>
+      </c>
+      <c r="B41">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>105</v>
+      </c>
+      <c r="B42">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>115</v>
+      </c>
+      <c r="B43">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>130</v>
+      </c>
+      <c r="B44">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="43"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="43"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="43">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="43"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="47" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>315</v>
+      </c>
+      <c r="B54" s="34"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>12</v>
+      </c>
+      <c r="B58" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>75</v>
+      </c>
+      <c r="B62" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>130</v>
+      </c>
+      <c r="B65" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f>(A58*A62+A59*A65)/SUM(A58:A59)</f>
+        <v>108</v>
+      </c>
+      <c r="B68" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f>A68-A49</f>
+        <v>85</v>
+      </c>
+      <c r="B71" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="B77" s="38"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="48" t="s">
+        <v>269</v>
+      </c>
+      <c r="B81" s="49"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="36">
+        <f>AVERAGE(0.56,0.7)</f>
+        <v>0.63</v>
+      </c>
+      <c r="B82" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="42">
+        <f>AVERAGE(0.8,0.83)</f>
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="B83" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="34">
+        <f>AVERAGE(0.9,0.985)</f>
+        <v>0.9425</v>
+      </c>
+      <c r="B84" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f>1/A83</f>
+        <v>1.2269938650306749</v>
+      </c>
+      <c r="B89" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f>1/A74</f>
+        <v>0.4</v>
+      </c>
+      <c r="B92" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="50">
+        <f>(A89-A92)/A89</f>
+        <v>0.67399999999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -52937,16 +56496,18 @@
       <c r="A2" t="s">
         <v>303</v>
       </c>
-      <c r="B2" s="44">
-        <v>0.73</v>
+      <c r="B2" s="51">
+        <f>'Low Temp Heat'!A95</f>
+        <v>0.67399999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="45">
-        <v>0.32</v>
+      <c r="B3" s="51">
+        <f>'Med-High Temp Heat'!A39</f>
+        <v>0.22851035061589922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>